<commit_message>
Add new models DNN/MLP, LSTM and RNN for dataset one month
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>